<commit_message>
Added engine weight in excel
</commit_message>
<xml_diff>
--- a/ClassII_Weight_Estimation/Weight Balance/CG calcs.xlsx
+++ b/ClassII_Weight_Estimation/Weight Balance/CG calcs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\16266\OneDrive - Cal Poly\Documents\Weight Balance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\16266\OneDrive - Cal Poly\Documents\GitHub\443_design_problem\ClassII_Weight_Estimation\Weight Balance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C9C08C68-0E04-448B-8C8D-A55D21FC1B22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3ED168E-F020-485F-9A7C-E08C3EF6C11D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12710" yWindow="0" windowWidth="12980" windowHeight="13770" activeTab="1" xr2:uid="{59DD35D0-A79A-45B2-8D31-F1AE4E911AEB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{59DD35D0-A79A-45B2-8D31-F1AE4E911AEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Empty Weight" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="52">
   <si>
     <t>Component</t>
   </si>
@@ -88,18 +88,6 @@
     <t>Baggage</t>
   </si>
   <si>
-    <t>Sum</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Running Total</t>
-  </si>
-  <si>
-    <t>Count</t>
-  </si>
-  <si>
     <t>Number</t>
   </si>
   <si>
@@ -221,6 +209,12 @@
   </si>
   <si>
     <t>C.G.</t>
+  </si>
+  <si>
+    <t>Forward CG Calcs</t>
+  </si>
+  <si>
+    <t>Aft CG Calcs</t>
   </si>
 </sst>
 </file>
@@ -284,7 +278,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -305,6 +299,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -644,7 +641,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -662,16 +659,16 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -679,7 +676,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -694,7 +691,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -709,10 +706,14 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+        <v>42</v>
+      </c>
+      <c r="C4" s="3">
+        <v>593.13</v>
+      </c>
+      <c r="D4" s="3">
+        <v>593.13</v>
+      </c>
       <c r="E4" s="4"/>
       <c r="F4">
         <f t="shared" si="0"/>
@@ -724,7 +725,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -739,7 +740,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -751,12 +752,14 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" s="3"/>
+        <v>45</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0</v>
+      </c>
       <c r="D7" s="3"/>
       <c r="E7" s="4"/>
       <c r="F7">
@@ -766,12 +769,14 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C8" s="3"/>
+        <v>47</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0</v>
+      </c>
       <c r="D8" s="3"/>
       <c r="F8">
         <f t="shared" si="0"/>
@@ -780,11 +785,11 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="E10" t="s">
-        <v>53</v>
-      </c>
-      <c r="F10" t="e" cm="1">
+        <v>49</v>
+      </c>
+      <c r="F10" cm="1">
         <f t="array" ref="F10">SUM(F2:F8/SUM(C2:C8))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -794,10 +799,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41428DCE-B4DC-4B74-93FB-17A21D3B8CE9}">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -813,25 +818,25 @@
   <sheetData>
     <row r="1" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -839,7 +844,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C2" s="7">
         <v>2414.1</v>
@@ -852,10 +857,10 @@
         <v>4103.9699999999993</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -863,7 +868,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C3" s="7">
         <v>166.9</v>
@@ -872,14 +877,14 @@
         <v>2.4</v>
       </c>
       <c r="E3" s="7">
-        <f t="shared" ref="E3:E24" si="0">C3*D3</f>
+        <f t="shared" ref="E3:E5" si="0">C3*D3</f>
         <v>400.56</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -887,7 +892,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C4" s="7">
         <v>35.6</v>
@@ -900,10 +905,10 @@
         <v>21.36</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -911,7 +916,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C5" s="7">
         <v>445</v>
@@ -924,450 +929,484 @@
         <v>756.5</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="2">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="1">
-        <v>3061.6</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="1">
-        <v>1.7</v>
-      </c>
-      <c r="G6" s="1">
-        <v>17.600000000000001</v>
-      </c>
+      <c r="A6" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C7" s="1">
-        <v>311.5</v>
-      </c>
-      <c r="D7" s="1">
+        <v>3061.6</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="1">
         <v>1.7</v>
       </c>
-      <c r="E7" s="1">
-        <f t="shared" si="0"/>
-        <v>529.54999999999995</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>19</v>
+      <c r="G7" s="1">
+        <v>17.600000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C8" s="1">
-        <v>3373.1</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="1">
+        <v>311.5</v>
+      </c>
+      <c r="D8" s="1">
         <v>1.7</v>
       </c>
-      <c r="G8" s="1">
-        <v>17.3</v>
+      <c r="E8" s="1">
+        <f>C8*D8</f>
+        <v>529.54999999999995</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C9" s="1">
-        <v>756.5</v>
-      </c>
-      <c r="D9" s="1">
+        <v>3373.1</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="1">
         <v>1.7</v>
       </c>
-      <c r="E9" s="1">
-        <f t="shared" si="0"/>
-        <v>1286.05</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>19</v>
+      <c r="G9" s="1">
+        <v>17.3</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C10" s="1">
-        <v>4129.6000000000004</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="1">
+        <v>756.5</v>
+      </c>
+      <c r="D10" s="1">
         <v>1.7</v>
       </c>
-      <c r="G10" s="1">
-        <v>16.7</v>
+      <c r="E10" s="1">
+        <f>C10*D10</f>
+        <v>1286.05</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="C11" s="1">
-        <v>356</v>
-      </c>
-      <c r="D11" s="1">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E11" s="1">
-        <f t="shared" si="0"/>
-        <v>783.2</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>19</v>
+        <v>4129.6000000000004</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1.7</v>
+      </c>
+      <c r="G11" s="1">
+        <v>16.7</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="C12" s="1">
-        <v>4485.6000000000004</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" s="1">
-        <v>1.8</v>
-      </c>
-      <c r="G12" s="1">
-        <v>19.7</v>
+        <v>356</v>
+      </c>
+      <c r="D12" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E12" s="1">
+        <f>C12*D12</f>
+        <v>783.2</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C13" s="1">
-        <v>146.80000000000001</v>
-      </c>
-      <c r="D13" s="1">
-        <v>2.4</v>
-      </c>
-      <c r="E13" s="1">
-        <f t="shared" si="0"/>
-        <v>352.32</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>19</v>
+        <v>4485.6000000000004</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="G13" s="1">
+        <v>19.7</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="1">
+        <v>146.80000000000001</v>
+      </c>
+      <c r="D14" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="E14" s="1">
+        <f>C14*D14</f>
+        <v>352.32</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="2">
         <v>13</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="1">
+      <c r="B15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="1">
         <v>4632.3999999999996</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" s="1">
-        <f>SUM(E2:E13)</f>
+      <c r="D15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="1">
+        <f>SUM(E2:E14)</f>
         <v>8233.51</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F15" s="1">
         <v>1.8</v>
       </c>
-      <c r="G14" s="1">
+      <c r="G15" s="1">
         <v>21.3</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-    </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="2">
-        <v>5</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="1">
-        <v>3061.6</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F16" s="1">
-        <v>1.7</v>
-      </c>
-      <c r="G16" s="1">
-        <v>17.600000000000001</v>
-      </c>
+      <c r="A16" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C17" s="1">
-        <v>146.80000000000001</v>
-      </c>
-      <c r="D17" s="1">
-        <v>2.4</v>
-      </c>
-      <c r="E17" s="1">
-        <f t="shared" si="0"/>
-        <v>352.32</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>19</v>
+        <v>3061.6</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1.7</v>
+      </c>
+      <c r="G17" s="1">
+        <v>17.600000000000001</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C18" s="1">
-        <v>3208.4</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F18" s="1">
-        <v>1.8</v>
-      </c>
-      <c r="G18" s="1">
-        <v>20</v>
+        <v>146.80000000000001</v>
+      </c>
+      <c r="D18" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="E18" s="1">
+        <f>C18*D18</f>
+        <v>352.32</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="C19" s="1">
-        <v>356</v>
-      </c>
-      <c r="D19" s="1">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E19" s="1">
-        <f t="shared" si="0"/>
-        <v>783.2</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>19</v>
+        <v>3208.4</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="G19" s="1">
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="C20" s="1">
-        <v>3564.4</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F20" s="1">
-        <v>1.8</v>
-      </c>
-      <c r="G20" s="1">
-        <v>23.5</v>
+        <v>356</v>
+      </c>
+      <c r="D20" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E20" s="1">
+        <f>C20*D20</f>
+        <v>783.2</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="C21" s="1">
-        <v>756.5</v>
-      </c>
-      <c r="D21" s="1">
-        <v>1.7</v>
-      </c>
-      <c r="E21" s="1">
-        <f t="shared" si="0"/>
-        <v>1286.05</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>19</v>
+        <v>3564.4</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F21" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="G21" s="1">
+        <v>23.5</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="C22" s="1">
-        <v>4320.8999999999996</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F22" s="1">
-        <v>1.8</v>
-      </c>
-      <c r="G22" s="1">
-        <v>21.8</v>
+        <v>756.5</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1.7</v>
+      </c>
+      <c r="E22" s="1">
+        <f>C22*D22</f>
+        <v>1286.05</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="C23" s="1">
-        <v>311.5</v>
-      </c>
-      <c r="D23" s="1">
-        <v>1.7</v>
-      </c>
-      <c r="E23" s="1">
-        <f t="shared" si="0"/>
-        <v>529.54999999999995</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>19</v>
+        <v>4320.8999999999996</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="G23" s="1">
+        <v>21.8</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
+        <v>20</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="1">
+        <v>311.5</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1.7</v>
+      </c>
+      <c r="E24" s="1">
+        <f>C24*D24</f>
+        <v>529.54999999999995</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25" s="2">
         <v>21</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C24" s="1">
+      <c r="B25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="1">
         <v>4632.3999999999996</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F24" s="1">
+      <c r="D25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25" s="1">
         <v>1.8</v>
       </c>
-      <c r="G24" s="1">
+      <c r="G25" s="1">
         <v>21.3</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="A16:G16"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="5e3388d9-314e-4294-86c7-b13e3e1771a6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DD955F58912B654AAA143FB6F23867BF" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ca35ef2c79184dece2382fe10a86ecc2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5e3388d9-314e-4294-86c7-b13e3e1771a6" xmlns:ns4="b7f6fc4a-4dd4-4733-a317-024af99a3eac" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="11badb3ba1486ac4ed64eef28c55e54c" ns3:_="" ns4:_="">
     <xsd:import namespace="5e3388d9-314e-4294-86c7-b13e3e1771a6"/>
@@ -1620,24 +1659,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84793EFF-49C1-4883-A0FB-581B72B07948}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="b7f6fc4a-4dd4-4733-a317-024af99a3eac"/>
+    <ds:schemaRef ds:uri="5e3388d9-314e-4294-86c7-b13e3e1771a6"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="5e3388d9-314e-4294-86c7-b13e3e1771a6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78904E1D-471D-4B0D-997C-93DA4375DA7A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{93CDCB7F-8648-4905-9D51-EA330003B102}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1654,29 +1701,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78904E1D-471D-4B0D-997C-93DA4375DA7A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84793EFF-49C1-4883-A0FB-581B72B07948}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="b7f6fc4a-4dd4-4733-a317-024af99a3eac"/>
-    <ds:schemaRef ds:uri="5e3388d9-314e-4294-86c7-b13e3e1771a6"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added more stuff to CG stuff
</commit_message>
<xml_diff>
--- a/ClassII_Weight_Estimation/Weight Balance/CG calcs.xlsx
+++ b/ClassII_Weight_Estimation/Weight Balance/CG calcs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\16266\OneDrive - Cal Poly\Documents\GitHub\443_design_problem\ClassII_Weight_Estimation\Weight Balance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C345CED-9996-4227-9656-F7991AAABB2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBFE13EB-6075-4939-9B6B-B70FDF6EE65F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{59DD35D0-A79A-45B2-8D31-F1AE4E911AEB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{59DD35D0-A79A-45B2-8D31-F1AE4E911AEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Empty Weight" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="63">
   <si>
     <t>Component</t>
   </si>
@@ -94,9 +94,6 @@
     <t>W.x</t>
   </si>
   <si>
-    <t>CG Position</t>
-  </si>
-  <si>
     <t>%cma</t>
   </si>
   <si>
@@ -118,9 +115,6 @@
     <t>minimum operating weight</t>
   </si>
   <si>
-    <t>pilot</t>
-  </si>
-  <si>
     <t>partial weight (5+6)</t>
   </si>
   <si>
@@ -190,9 +184,6 @@
     <t>Propeller</t>
   </si>
   <si>
-    <t>Empanage</t>
-  </si>
-  <si>
     <t>Main Gear</t>
   </si>
   <si>
@@ -215,6 +206,48 @@
   </si>
   <si>
     <t>I think we need to analyize different payload configs? No way we have time to do this right now but manybe eventually</t>
+  </si>
+  <si>
+    <t>Assumed 42%</t>
+  </si>
+  <si>
+    <t>Component 8</t>
+  </si>
+  <si>
+    <t>Nacelles</t>
+  </si>
+  <si>
+    <t>Component 9</t>
+  </si>
+  <si>
+    <t>Tail Boom</t>
+  </si>
+  <si>
+    <t>Assume 40%</t>
+  </si>
+  <si>
+    <t>Assume 50%</t>
+  </si>
+  <si>
+    <t>Assumed by oilver</t>
+  </si>
+  <si>
+    <t>Hor. Tail</t>
+  </si>
+  <si>
+    <t>Vert Tail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pilot </t>
+  </si>
+  <si>
+    <t>CG Position [ft]</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Volume of wing (US Gal)</t>
   </si>
 </sst>
 </file>
@@ -638,10 +671,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A96154D2-D2DA-438D-B5A0-7CF0FCADAAC6}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -653,60 +686,70 @@
     <col min="5" max="5" width="7.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" s="4"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="F1" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="4"/>
+      <c r="D2" s="3">
+        <v>800</v>
+      </c>
+      <c r="E2" s="4">
+        <v>13.972</v>
+      </c>
       <c r="F2">
         <f>D2*E2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+        <v>11177.6</v>
+      </c>
+      <c r="H2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="4"/>
+      <c r="E3" s="4">
+        <f>(142.96/12)</f>
+        <v>11.913333333333334</v>
+      </c>
       <c r="F3">
-        <f t="shared" ref="F3:F8" si="0">D3*E3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+        <f t="shared" ref="F3:F9" si="0">D3*E3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C4" s="3">
         <v>593.13</v>
@@ -714,82 +757,172 @@
       <c r="D4" s="3">
         <v>593.13</v>
       </c>
-      <c r="E4" s="4"/>
+      <c r="E4" s="4">
+        <v>5.0570000000000004</v>
+      </c>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+        <v>2999.4584100000002</v>
+      </c>
+      <c r="H4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="4"/>
+      <c r="E5" s="4">
+        <f>18.97/12</f>
+        <v>1.5808333333333333</v>
+      </c>
       <c r="F5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="4"/>
+      <c r="E6" s="4">
+        <v>31.734999999999999</v>
+      </c>
       <c r="F6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
-        <v>37</v>
-      </c>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" s="3">
-        <v>0</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="C7" s="3"/>
       <c r="D7" s="3"/>
-      <c r="E7" s="4"/>
+      <c r="E7" s="4">
+        <v>31.742999999999999</v>
+      </c>
       <c r="F7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C8" s="3">
         <v>0</v>
       </c>
       <c r="D8" s="3"/>
+      <c r="E8" s="4">
+        <f>174.37/12</f>
+        <v>14.530833333333334</v>
+      </c>
       <c r="F8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="E10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F10" cm="1">
-        <f t="array" ref="F10">SUM(F2:F8/SUM(C2:C8))</f>
-        <v>0</v>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9">
+        <f>48.09/12</f>
+        <v>4.0075000000000003</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10">
+        <f>57.18/12</f>
+        <v>4.7649999999999997</v>
+      </c>
+      <c r="F10">
+        <f t="shared" ref="F10" si="1">D10*E10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11">
+        <f>305.53/12</f>
+        <v>25.46083333333333</v>
+      </c>
+      <c r="F11">
+        <f t="shared" ref="F11" si="2">D11*E11</f>
+        <v>0</v>
+      </c>
+      <c r="H11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="E13" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" cm="1">
+        <f t="array" ref="F13">SUM(F2:F9/SUM(C2:C9))</f>
+        <v>23.90210984101293</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="C21">
+        <v>198.1</v>
       </c>
     </row>
   </sheetData>
@@ -801,8 +934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41428DCE-B4DC-4B74-93FB-17A21D3B8CE9}">
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -810,13 +943,13 @@
     <col min="1" max="1" width="8.6328125" customWidth="1"/>
     <col min="2" max="2" width="25.6328125" customWidth="1"/>
     <col min="3" max="3" width="6.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.54296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.36328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.6328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>8</v>
       </c>
@@ -824,19 +957,19 @@
         <v>9</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>11</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
@@ -844,23 +977,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="7">
-        <v>2414.1</v>
-      </c>
-      <c r="D2" s="7">
-        <v>1.7</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
       <c r="E2" s="7">
         <f>C2*D2</f>
-        <v>4103.9699999999993</v>
+        <v>0</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
@@ -868,23 +997,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="7">
-        <v>166.9</v>
-      </c>
-      <c r="D3" s="7">
-        <v>2.4</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
       <c r="E3" s="7">
         <f t="shared" ref="E3:E5" si="0">C3*D3</f>
-        <v>400.56</v>
+        <v>0</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
@@ -892,23 +1017,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="7">
-        <v>35.6</v>
-      </c>
-      <c r="D4" s="7">
-        <v>0.6</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
       <c r="E4" s="7">
         <f t="shared" si="0"/>
-        <v>21.36</v>
+        <v>0</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
@@ -916,31 +1037,27 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="7">
-        <v>445</v>
-      </c>
-      <c r="D5" s="7">
-        <v>1.7</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
       <c r="E5" s="7">
         <f t="shared" si="0"/>
-        <v>756.5</v>
+        <v>0</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
@@ -954,16 +1071,12 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="1">
-        <v>3061.6</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F7" s="1">
         <v>1.7</v>
@@ -977,23 +1090,23 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="C8" s="1">
-        <v>311.5</v>
+        <v>220</v>
       </c>
       <c r="D8" s="1">
-        <v>1.7</v>
+        <v>11.977</v>
       </c>
       <c r="E8" s="1">
         <f>C8*D8</f>
-        <v>529.54999999999995</v>
+        <v>2634.94</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
@@ -1001,16 +1114,15 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C9" s="1">
-        <v>3373.1</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>14</v>
-      </c>
+        <f>C7+C8</f>
+        <v>220</v>
+      </c>
+      <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F9" s="1">
         <v>1.7</v>
@@ -1024,23 +1136,23 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C10" s="1">
-        <v>756.5</v>
+        <v>220</v>
       </c>
       <c r="D10" s="1">
-        <v>1.7</v>
+        <v>16.454000000000001</v>
       </c>
       <c r="E10" s="1">
         <f>C10*D10</f>
-        <v>1286.05</v>
+        <v>3619.88</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
@@ -1048,16 +1160,15 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C11" s="1">
-        <v>4129.6000000000004</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>14</v>
-      </c>
+        <f>C9+C10</f>
+        <v>440</v>
+      </c>
+      <c r="D11" s="1"/>
       <c r="E11" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F11" s="1">
         <v>1.7</v>
@@ -1071,23 +1182,21 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C12" s="1">
-        <v>356</v>
-      </c>
-      <c r="D12" s="1">
-        <v>2.2000000000000002</v>
-      </c>
+        <v>3500</v>
+      </c>
+      <c r="D12" s="1"/>
       <c r="E12" s="1">
         <f>C12*D12</f>
-        <v>783.2</v>
+        <v>0</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
@@ -1095,16 +1204,15 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C13" s="1">
-        <v>4485.6000000000004</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>14</v>
-      </c>
+        <f>C11+C12</f>
+        <v>3940</v>
+      </c>
+      <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F13" s="1">
         <v>1.8</v>
@@ -1118,23 +1226,19 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="1">
-        <v>146.80000000000001</v>
-      </c>
-      <c r="D14" s="1">
-        <v>2.4</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
       <c r="E14" s="1">
         <f>C14*D14</f>
-        <v>352.32</v>
+        <v>0</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
@@ -1142,17 +1246,16 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C15" s="1">
-        <v>4632.3999999999996</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>14</v>
-      </c>
+        <f>SUM(C7:C14)</f>
+        <v>8540</v>
+      </c>
+      <c r="D15" s="1"/>
       <c r="E15" s="1">
         <f>SUM(E2:E14)</f>
-        <v>8233.51</v>
+        <v>6254.82</v>
       </c>
       <c r="F15" s="1">
         <v>1.8</v>
@@ -1163,7 +1266,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -1177,17 +1280,11 @@
         <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="1">
-        <v>3061.6</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
       <c r="F17" s="1">
         <v>1.7</v>
       </c>
@@ -1200,23 +1297,16 @@
         <v>14</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="1">
-        <v>146.80000000000001</v>
-      </c>
-      <c r="D18" s="1">
-        <v>2.4</v>
-      </c>
-      <c r="E18" s="1">
-        <f>C18*D18</f>
-        <v>352.32</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
       <c r="F18" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
@@ -1224,17 +1314,11 @@
         <v>15</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="1">
-        <v>3208.4</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
       <c r="F19" s="1">
         <v>1.8</v>
       </c>
@@ -1247,23 +1331,16 @@
         <v>16</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="1">
-        <v>356</v>
-      </c>
-      <c r="D20" s="1">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E20" s="1">
-        <f>C20*D20</f>
-        <v>783.2</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
       <c r="F20" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
@@ -1271,17 +1348,11 @@
         <v>17</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" s="1">
-        <v>3564.4</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
       <c r="F21" s="1">
         <v>1.8</v>
       </c>
@@ -1296,21 +1367,14 @@
       <c r="B22" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C22" s="1">
-        <v>756.5</v>
-      </c>
-      <c r="D22" s="1">
-        <v>1.7</v>
-      </c>
-      <c r="E22" s="1">
-        <f>C22*D22</f>
-        <v>1286.05</v>
-      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
       <c r="F22" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
@@ -1318,17 +1382,11 @@
         <v>19</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C23" s="1">
-        <v>4320.8999999999996</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
       <c r="F23" s="1">
         <v>1.8</v>
       </c>
@@ -1343,21 +1401,14 @@
       <c r="B24" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C24" s="1">
-        <v>311.5</v>
-      </c>
-      <c r="D24" s="1">
-        <v>1.7</v>
-      </c>
-      <c r="E24" s="1">
-        <f>C24*D24</f>
-        <v>529.54999999999995</v>
-      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
       <c r="F24" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
@@ -1365,17 +1416,11 @@
         <v>21</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C25" s="1">
-        <v>4632.3999999999996</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
       <c r="F25" s="1">
         <v>1.8</v>
       </c>
@@ -1393,23 +1438,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="5e3388d9-314e-4294-86c7-b13e3e1771a6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DD955F58912B654AAA143FB6F23867BF" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ca35ef2c79184dece2382fe10a86ecc2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5e3388d9-314e-4294-86c7-b13e3e1771a6" xmlns:ns4="b7f6fc4a-4dd4-4733-a317-024af99a3eac" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="11badb3ba1486ac4ed64eef28c55e54c" ns3:_="" ns4:_="">
     <xsd:import namespace="5e3388d9-314e-4294-86c7-b13e3e1771a6"/>
@@ -1662,32 +1690,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84793EFF-49C1-4883-A0FB-581B72B07948}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="b7f6fc4a-4dd4-4733-a317-024af99a3eac"/>
-    <ds:schemaRef ds:uri="5e3388d9-314e-4294-86c7-b13e3e1771a6"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78904E1D-471D-4B0D-997C-93DA4375DA7A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="5e3388d9-314e-4294-86c7-b13e3e1771a6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{93CDCB7F-8648-4905-9D51-EA330003B102}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1704,4 +1724,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78904E1D-471D-4B0D-997C-93DA4375DA7A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84793EFF-49C1-4883-A0FB-581B72B07948}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="b7f6fc4a-4dd4-4733-a317-024af99a3eac"/>
+    <ds:schemaRef ds:uri="5e3388d9-314e-4294-86c7-b13e3e1771a6"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Revert "Merge branch 'main' of https://github.com/tchen2021/443_design_problem"
This reverts commit df52dfdeae05172a2585eac86738e719ed7f4a49, reversing
changes made to 5624c7c38503b8a3c8a5118a370782392cb9fcd5.
</commit_message>
<xml_diff>
--- a/ClassII_Weight_Estimation/Weight Balance/CG calcs.xlsx
+++ b/ClassII_Weight_Estimation/Weight Balance/CG calcs.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\16266\OneDrive - Cal Poly\Documents\GitHub\443_design_problem\ClassII_Weight_Estimation\Weight Balance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C345CED-9996-4227-9656-F7991AAABB2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11D11EEB-BEEF-4101-8D48-23DC545AB761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{59DD35D0-A79A-45B2-8D31-F1AE4E911AEB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{59DD35D0-A79A-45B2-8D31-F1AE4E911AEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Empty Weight" sheetId="1" r:id="rId1"/>
     <sheet name="CG_Envelope" sheetId="2" r:id="rId2"/>
+    <sheet name="Landing Gear" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,30 +37,83 @@
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Shuo Chen</author>
+  </authors>
+  <commentList>
+    <comment ref="E5" authorId="0" shapeId="0" xr:uid="{F369CCC9-EF30-4DEA-B611-F525C212FF50}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Shuo Chen:
+CG location very sensitive to this
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E6" authorId="0" shapeId="0" xr:uid="{C46A1D5A-A700-4B2D-9F3A-E695F7A27263}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Shuo Chen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+CG sensitive
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E8" authorId="0" shapeId="0" xr:uid="{ACA19C8B-D27C-4CB6-814E-1C6DECE0D3F2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Shuo Chen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Break down somehome to nose and main</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="95">
   <si>
     <t>Component</t>
   </si>
@@ -94,9 +148,6 @@
     <t>W.x</t>
   </si>
   <si>
-    <t>CG Position</t>
-  </si>
-  <si>
     <t>%cma</t>
   </si>
   <si>
@@ -118,9 +169,6 @@
     <t>minimum operating weight</t>
   </si>
   <si>
-    <t>pilot</t>
-  </si>
-  <si>
     <t>partial weight (5+6)</t>
   </si>
   <si>
@@ -184,15 +232,6 @@
     <t>Fuselage</t>
   </si>
   <si>
-    <t>Engine</t>
-  </si>
-  <si>
-    <t>Propeller</t>
-  </si>
-  <si>
-    <t>Empanage</t>
-  </si>
-  <si>
     <t>Main Gear</t>
   </si>
   <si>
@@ -205,9 +244,6 @@
     <t>W.X</t>
   </si>
   <si>
-    <t>C.G.</t>
-  </si>
-  <si>
     <t>Forward CG Calcs</t>
   </si>
   <si>
@@ -215,13 +251,163 @@
   </si>
   <si>
     <t>I think we need to analyize different payload configs? No way we have time to do this right now but manybe eventually</t>
+  </si>
+  <si>
+    <t>Assumed 42%</t>
+  </si>
+  <si>
+    <t>Component 8</t>
+  </si>
+  <si>
+    <t>Nacelles</t>
+  </si>
+  <si>
+    <t>Component 9</t>
+  </si>
+  <si>
+    <t>Tail Boom</t>
+  </si>
+  <si>
+    <t>Assume 40%</t>
+  </si>
+  <si>
+    <t>Assume 50%</t>
+  </si>
+  <si>
+    <t>Assumed by oilver</t>
+  </si>
+  <si>
+    <t>Vert Tail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pilot </t>
+  </si>
+  <si>
+    <t>CG Position [ft]</t>
+  </si>
+  <si>
+    <t>Volume of wing (US Gal)</t>
+  </si>
+  <si>
+    <t>Total Length</t>
+  </si>
+  <si>
+    <t>MAC_length</t>
+  </si>
+  <si>
+    <t>x_MAC</t>
+  </si>
+  <si>
+    <t>Emp</t>
+  </si>
+  <si>
+    <t>C.G. %MAC</t>
+  </si>
+  <si>
+    <t>x_CG</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Landing Gear</t>
+  </si>
+  <si>
+    <t>Engine/</t>
+  </si>
+  <si>
+    <t>Propulsion Group</t>
+  </si>
+  <si>
+    <t>Wing Move</t>
+  </si>
+  <si>
+    <t>Fuselage Move</t>
+  </si>
+  <si>
+    <t>Assumed 35%</t>
+  </si>
+  <si>
+    <t>Wing Margin</t>
+  </si>
+  <si>
+    <t>Landing Gear Margin</t>
+  </si>
+  <si>
+    <t>Fuselage Margin</t>
+  </si>
+  <si>
+    <t>Note for CAD</t>
+  </si>
+  <si>
+    <t>Move Wing forward 2 feet</t>
+  </si>
+  <si>
+    <t>min fuel determined with SFC for 75% power for 30 min flight</t>
+  </si>
+  <si>
+    <t>% MAC</t>
+  </si>
+  <si>
+    <t>Weight [lb]</t>
+  </si>
+  <si>
+    <t>X Location [ft]</t>
+  </si>
+  <si>
+    <t>Empty Weight</t>
+  </si>
+  <si>
+    <t>Margin</t>
+  </si>
+  <si>
+    <t>EWF</t>
+  </si>
+  <si>
+    <t>Class I EWF</t>
+  </si>
+  <si>
+    <t>Operating EW</t>
+  </si>
+  <si>
+    <t>F CG % MAC</t>
+  </si>
+  <si>
+    <t>AFT CG % MAC</t>
+  </si>
+  <si>
+    <t>X F CG [ft]</t>
+  </si>
+  <si>
+    <t>X AFT CG [ft]</t>
+  </si>
+  <si>
+    <t>Step 2:</t>
+  </si>
+  <si>
+    <t>Step 1:</t>
+  </si>
+  <si>
+    <t>Line % MAC</t>
+  </si>
+  <si>
+    <t>x  line</t>
+  </si>
+  <si>
+    <t>Step 3:</t>
+  </si>
+  <si>
+    <t>Fuel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -245,8 +431,47 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -265,8 +490,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -274,19 +511,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -304,9 +554,78 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -319,6 +638,1082 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>CG_Envelope!$J$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>W [lb]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>CG_Envelope!$I$7:$I$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>17.418739686781194</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19.615344414614391</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27.814132425568534</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24.1478</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20.810764298709032</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20.810764298709032</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>17.418739686781194</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>CG_Envelope!$J$7:$J$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0" formatCode="0.00">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8720</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11593.52</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8136.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5220</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5220</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.00">
+                  <c:v>5000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9363-4E5C-8780-3FB73D8D93B0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="406306832"/>
+        <c:axId val="406306352"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="406306832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="30"/>
+          <c:min val="15"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US">
+                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t>%</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0">
+                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t> MAC</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US">
+                  <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                  <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.47623490813648295"/>
+              <c:y val="0.87405074365704283"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                  <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="406306352"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="406306352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="5000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US">
+                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t>Weight</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0">
+                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t> [lb]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US">
+                  <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                  <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="2.5000000000000001E-2"/>
+              <c:y val="0.34088327500729076"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                  <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="406306832"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>184977</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>64051</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>505238</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>73990</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE340039-29B2-402E-56A8-82E0AA0925CF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -637,11 +2032,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A96154D2-D2DA-438D-B5A0-7CF0FCADAAC6}">
-  <dimension ref="A1:F10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A96154D2-D2DA-438D-B5A0-7CF0FCADAAC6}">
+  <dimension ref="A1:T26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -651,325 +2046,713 @@
     <col min="3" max="3" width="8.6328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.453125" customWidth="1"/>
     <col min="5" max="5" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.6328125" customWidth="1"/>
+    <col min="19" max="19" width="12" customWidth="1"/>
+    <col min="20" max="20" width="13.453125" customWidth="1"/>
+    <col min="21" max="21" width="14.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="4"/>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="9"/>
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="F1" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="R1" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="S1" s="20"/>
+      <c r="T1" s="20"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="4"/>
-      <c r="F2">
+      <c r="B2" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12">
+        <f>817*O2</f>
+        <v>1634</v>
+      </c>
+      <c r="E2" s="9">
+        <f>13.972 + H26</f>
+        <v>12.972</v>
+      </c>
+      <c r="F2" s="13">
         <f>D2*E2</f>
+        <v>21196.248</v>
+      </c>
+      <c r="H2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" s="3">
+        <v>13.972</v>
+      </c>
+      <c r="N2" t="s">
+        <v>71</v>
+      </c>
+      <c r="O2">
+        <v>2</v>
+      </c>
+      <c r="R2" s="21" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+      <c r="S2" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="T2" s="22" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="4"/>
-      <c r="F3">
-        <f t="shared" ref="F3:F8" si="0">D3*E3</f>
+      <c r="B3" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12">
+        <f>497*O3</f>
+        <v>1491</v>
+      </c>
+      <c r="E3" s="9">
+        <f>(146/12)+I26</f>
+        <v>12.166666666666666</v>
+      </c>
+      <c r="F3" s="13">
+        <f t="shared" ref="F3:F10" si="0">D3*E3</f>
+        <v>18140.5</v>
+      </c>
+      <c r="H3" t="s">
+        <v>70</v>
+      </c>
+      <c r="N3" t="s">
+        <v>73</v>
+      </c>
+      <c r="O3">
+        <v>3</v>
+      </c>
+      <c r="R3" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="S3" s="18">
+        <v>1634</v>
+      </c>
+      <c r="T3" s="23">
+        <v>12.972</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A4" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="12">
+        <v>593.13</v>
+      </c>
+      <c r="D4" s="12">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4" s="3">
-        <v>593.13</v>
-      </c>
-      <c r="D4" s="3">
-        <v>593.13</v>
-      </c>
-      <c r="E4" s="4"/>
-      <c r="F4">
+      <c r="E4" s="9">
+        <v>5.5</v>
+      </c>
+      <c r="F4" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
+      <c r="H4" t="s">
+        <v>52</v>
+      </c>
+      <c r="R4" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="S4" s="18">
+        <v>1491</v>
+      </c>
+      <c r="T4" s="23">
+        <v>12.166666666666666</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="4"/>
-      <c r="F5">
+      <c r="B5" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29">
+        <v>928</v>
+      </c>
+      <c r="E5" s="30">
+        <v>5.5</v>
+      </c>
+      <c r="F5" s="31">
+        <f t="shared" si="0"/>
+        <v>5104</v>
+      </c>
+      <c r="H5" t="s">
+        <v>53</v>
+      </c>
+      <c r="R5" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="S5" s="18">
+        <v>928</v>
+      </c>
+      <c r="T5" s="23">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A6" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29">
+        <v>140</v>
+      </c>
+      <c r="E6" s="30">
+        <f>(31.735+31.743)/2</f>
+        <v>31.738999999999997</v>
+      </c>
+      <c r="F6" s="31">
+        <f>D6*E6</f>
+        <v>4443.46</v>
+      </c>
+      <c r="R6" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="S6" s="18">
+        <v>140</v>
+      </c>
+      <c r="T6" s="23">
+        <v>31.738999999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A7" s="13"/>
+      <c r="B7" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="9">
+        <v>31.742999999999999</v>
+      </c>
+      <c r="F7" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="4"/>
-      <c r="F6">
+      <c r="R7" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="S7" s="18">
+        <v>225</v>
+      </c>
+      <c r="T7" s="23">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A8" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13">
+        <f>225</f>
+        <v>225</v>
+      </c>
+      <c r="E8" s="13">
+        <v>10.7</v>
+      </c>
+      <c r="F8" s="13">
+        <f t="shared" si="0"/>
+        <v>2407.5</v>
+      </c>
+      <c r="N8" t="s">
+        <v>72</v>
+      </c>
+      <c r="O8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A9" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="12">
+        <v>0</v>
+      </c>
+      <c r="D9" s="12"/>
+      <c r="E9" s="9">
+        <f>174.37/12</f>
+        <v>14.530833333333334</v>
+      </c>
+      <c r="F9" s="13">
+        <f>D9*E9</f>
+        <v>0</v>
+      </c>
+      <c r="R9" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="S9" s="18">
+        <v>4418</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A10" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="12">
+        <v>0</v>
+      </c>
+      <c r="D10" s="12"/>
+      <c r="E10" s="13">
+        <f>48.09/12</f>
+        <v>4.0075000000000003</v>
+      </c>
+      <c r="F10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" s="3">
+      <c r="R10" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="S10" s="14">
+        <f>5000</f>
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A11" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="12">
         <v>0</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="4"/>
-      <c r="F7">
-        <f t="shared" si="0"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="13">
+        <f>57.18/12</f>
+        <v>4.7649999999999997</v>
+      </c>
+      <c r="F11" s="13">
+        <f t="shared" ref="F11" si="1">D11*E11</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C8" s="3">
+      <c r="R11" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="S11" s="18">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A12" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="12">
         <v>0</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="F8">
-        <f t="shared" si="0"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="13">
+        <f>305.53/12</f>
+        <v>25.46083333333333</v>
+      </c>
+      <c r="F12" s="13">
+        <f>D12*E12</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="E10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F10" cm="1">
-        <f t="array" ref="F10">SUM(F2:F8/SUM(C2:C8))</f>
+      <c r="H12" t="s">
+        <v>51</v>
+      </c>
+      <c r="R12" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="S12" s="18">
+        <f>0.51</f>
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A13" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13">
+        <f>SUM(C2:C12)</f>
+        <v>593.13</v>
+      </c>
+      <c r="D13" s="13">
+        <f>SUM(D2:D12)</f>
+        <v>4418</v>
+      </c>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="L13">
+        <f>12450*0.5034</f>
+        <v>6267.33</v>
+      </c>
+      <c r="R13" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="S13" s="25">
+        <f>S12-S11</f>
+        <v>0.16000000000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="E14" t="s">
+        <v>62</v>
+      </c>
+      <c r="F14">
+        <f>((SUM(F2:F12)/SUM(D2:D12)-B25)/C25)*100</f>
+        <v>17.832461044621795</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="E15" t="s">
+        <v>63</v>
+      </c>
+      <c r="F15">
+        <f>(SUM(F2:F12)/SUM(D2:D12))</f>
+        <v>11.609712086917156</v>
+      </c>
+      <c r="L15">
+        <f>4418-6260</f>
+        <v>-1842</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="S16">
+        <f>1842/12425</f>
+        <v>0.14824949698189135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A17" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="N17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A18" s="8">
+        <f>138.37/12</f>
+        <v>11.530833333333334</v>
+      </c>
+      <c r="B18" s="8">
+        <f>72.601/12</f>
+        <v>6.0500833333333333</v>
+      </c>
+      <c r="N18" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="C22">
+        <v>198.1</v>
+      </c>
+      <c r="Q22">
+        <f>4418/12500</f>
+        <v>0.35343999999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B24" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B25" s="8">
+        <f>138.37/12+H26</f>
+        <v>10.530833333333334</v>
+      </c>
+      <c r="C25" s="8">
+        <f>72.601/12</f>
+        <v>6.0500833333333333</v>
+      </c>
+      <c r="H25" t="s">
+        <v>68</v>
+      </c>
+      <c r="I25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="H26">
+        <v>-1</v>
+      </c>
+      <c r="I26">
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="R1:T1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41428DCE-B4DC-4B74-93FB-17A21D3B8CE9}">
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.6328125" customWidth="1"/>
     <col min="2" max="2" width="25.6328125" customWidth="1"/>
-    <col min="3" max="3" width="6.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" s="5" t="s">
+      <c r="C1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="5" t="s">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" s="6">
-        <v>1</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="7">
-        <v>2414.1</v>
-      </c>
-      <c r="D2" s="7">
-        <v>1.7</v>
-      </c>
-      <c r="E2" s="7">
+      <c r="C2" s="6">
+        <f>'Empty Weight'!D13</f>
+        <v>4418</v>
+      </c>
+      <c r="D2" s="6">
+        <f>'Empty Weight'!F15</f>
+        <v>11.609712086917156</v>
+      </c>
+      <c r="E2" s="6">
         <f>C2*D2</f>
-        <v>4103.9699999999993</v>
-      </c>
-      <c r="F2" s="7" t="s">
+        <v>51291.707999999999</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3" s="6">
-        <v>2</v>
-      </c>
-      <c r="B3" s="7" t="s">
+      <c r="C3" s="6">
+        <v>300</v>
+      </c>
+      <c r="D3" s="6">
+        <v>12.972</v>
+      </c>
+      <c r="E3" s="6">
+        <f t="shared" ref="E3:E5" si="0">C3*D3</f>
+        <v>3891.6</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="8">
+        <f>'Empty Weight'!B25</f>
+        <v>10.530833333333334</v>
+      </c>
+      <c r="J3" s="8">
+        <f>72.601/12</f>
+        <v>6.0500833333333333</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="7">
-        <v>166.9</v>
-      </c>
-      <c r="D3" s="7">
-        <v>2.4</v>
-      </c>
-      <c r="E3" s="7">
-        <f t="shared" ref="E3:E5" si="0">C3*D3</f>
-        <v>400.56</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A4" s="6">
-        <v>3</v>
-      </c>
-      <c r="B4" s="7" t="s">
+      <c r="C4" s="6">
+        <v>19.12</v>
+      </c>
+      <c r="D4" s="6">
+        <v>5.5</v>
+      </c>
+      <c r="E4" s="6">
+        <f t="shared" si="0"/>
+        <v>105.16000000000001</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="7">
-        <v>35.6</v>
-      </c>
-      <c r="D4" s="7">
-        <v>0.6</v>
-      </c>
-      <c r="E4" s="7">
+      <c r="C5" s="6">
+        <v>220</v>
+      </c>
+      <c r="D5" s="6">
+        <v>11.977</v>
+      </c>
+      <c r="E5" s="6">
         <f t="shared" si="0"/>
-        <v>21.36</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A5" s="6">
-        <v>4</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="7">
-        <v>445</v>
-      </c>
-      <c r="D5" s="7">
-        <v>1.7</v>
-      </c>
-      <c r="E5" s="7">
-        <f t="shared" si="0"/>
-        <v>756.5</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>14</v>
+        <v>2634.94</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="L5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A6" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
+      <c r="A6" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="I6" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="1">
-        <v>3061.6</v>
+        <v>17</v>
+      </c>
+      <c r="C7" s="16">
+        <f>ROUNDUP(SUM(C2:C5),-3)</f>
+        <v>5000</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="E7" s="1">
+        <f>SUM(E2:E5)</f>
+        <v>57923.408000000003</v>
       </c>
       <c r="F7" s="1">
-        <v>1.7</v>
+        <f>E7/C7</f>
+        <v>11.584681600000001</v>
       </c>
       <c r="G7" s="1">
-        <v>17.600000000000001</v>
+        <f>((F7-$I$3)/$J$3)*100</f>
+        <v>17.418739686781194</v>
+      </c>
+      <c r="I7" s="15">
+        <f>G7</f>
+        <v>17.418739686781194</v>
+      </c>
+      <c r="J7" s="17">
+        <f>C7</f>
+        <v>5000</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
@@ -977,23 +2760,34 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="C8" s="1">
-        <v>311.5</v>
+        <v>0</v>
       </c>
       <c r="D8" s="1">
-        <v>1.7</v>
+        <v>11.977</v>
       </c>
       <c r="E8" s="1">
         <f>C8*D8</f>
-        <v>529.54999999999995</v>
+        <v>0</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="I8" s="15">
+        <f>G13</f>
+        <v>19.615344414614391</v>
+      </c>
+      <c r="J8" s="15">
+        <f>C13</f>
+        <v>8720</v>
+      </c>
+      <c r="L8" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
@@ -1001,22 +2795,32 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C9" s="1">
-        <v>3373.1</v>
+        <f>C7+C8</f>
+        <v>5000</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F9" s="1">
-        <v>1.7</v>
+        <f>(E8+E7)/C9</f>
+        <v>11.584681600000001</v>
       </c>
       <c r="G9" s="1">
-        <v>17.3</v>
+        <f t="shared" ref="G9:G15" si="1">((F9-$I$3)/$J$3)*100</f>
+        <v>17.418739686781194</v>
+      </c>
+      <c r="I9" s="15">
+        <f>G21</f>
+        <v>27.814132425568534</v>
+      </c>
+      <c r="J9" s="15">
+        <v>11593.52</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
@@ -1024,23 +2828,30 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C10" s="1">
-        <v>756.5</v>
+        <v>220</v>
       </c>
       <c r="D10" s="1">
-        <v>1.7</v>
+        <v>16.454000000000001</v>
       </c>
       <c r="E10" s="1">
         <f>C10*D10</f>
-        <v>1286.05</v>
+        <v>3619.88</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="I10" s="15">
+        <v>24.1478</v>
+      </c>
+      <c r="J10" s="15">
+        <f>C21</f>
+        <v>8136.4</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
@@ -1048,22 +2859,33 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C11" s="1">
-        <v>4129.6000000000004</v>
+        <f>C9+C10</f>
+        <v>5220</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F11" s="1">
-        <v>1.7</v>
+        <f>SUM(E7,E8,E10)/C11</f>
+        <v>11.789901915708812</v>
       </c>
       <c r="G11" s="1">
-        <v>16.7</v>
+        <f>((F11-$I$3)/$J$3)*100</f>
+        <v>20.810764298709032</v>
+      </c>
+      <c r="I11" s="15">
+        <f>G19</f>
+        <v>20.810764298709032</v>
+      </c>
+      <c r="J11" s="15">
+        <f>C19</f>
+        <v>5220</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
@@ -1071,23 +2893,32 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C12" s="1">
-        <v>356</v>
+        <v>3500</v>
       </c>
       <c r="D12" s="1">
-        <v>2.2000000000000002</v>
+        <f>'Empty Weight'!F15</f>
+        <v>11.609712086917156</v>
       </c>
       <c r="E12" s="1">
         <f>C12*D12</f>
-        <v>783.2</v>
+        <v>40633.992304210049</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="I12" s="15">
+        <f>G11</f>
+        <v>20.810764298709032</v>
+      </c>
+      <c r="J12" s="15">
+        <f>C11</f>
+        <v>5220</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
@@ -1095,22 +2926,33 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C13" s="1">
-        <v>4485.6000000000004</v>
+        <f>C11+C12</f>
+        <v>8720</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F13" s="1">
-        <v>1.8</v>
+        <f>SUM(E8,E10,E12,E7)/C13</f>
+        <v>11.71757801653785</v>
       </c>
       <c r="G13" s="1">
-        <v>19.7</v>
+        <f t="shared" si="1"/>
+        <v>19.615344414614391</v>
+      </c>
+      <c r="I13" s="15">
+        <f>G7</f>
+        <v>17.418739686781194</v>
+      </c>
+      <c r="J13" s="17">
+        <f>C7</f>
+        <v>5000</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
@@ -1118,23 +2960,25 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C14" s="1">
-        <v>146.80000000000001</v>
+        <f>473*6.8-C3</f>
+        <v>2916.4</v>
       </c>
       <c r="D14" s="1">
-        <v>2.4</v>
+        <f>'Empty Weight'!E2</f>
+        <v>12.972</v>
       </c>
       <c r="E14" s="1">
         <f>C14*D14</f>
-        <v>352.32</v>
+        <v>37831.540800000002</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
@@ -1142,57 +2986,65 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C15" s="1">
-        <v>4632.3999999999996</v>
+        <f>C13+C14</f>
+        <v>11636.4</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E15" s="1">
-        <f>SUM(E2:E14)</f>
-        <v>8233.51</v>
+        <f>SUM(E7:E14)</f>
+        <v>140008.82110421004</v>
       </c>
       <c r="F15" s="1">
-        <v>1.8</v>
+        <f>E15/C15</f>
+        <v>12.031970463735352</v>
       </c>
       <c r="G15" s="1">
-        <v>21.3</v>
+        <f t="shared" si="1"/>
+        <v>24.811842212675057</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A16" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
+      <c r="A16" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C17" s="1">
-        <v>3061.6</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>14</v>
+        <f>C7</f>
+        <v>5000</v>
+      </c>
+      <c r="D17" s="1" t="str">
+        <f t="shared" ref="D17:G17" si="2">D7</f>
+        <v>-</v>
+      </c>
+      <c r="E17" s="1">
+        <f t="shared" si="2"/>
+        <v>57923.408000000003</v>
       </c>
       <c r="F17" s="1">
-        <v>1.7</v>
+        <f t="shared" si="2"/>
+        <v>11.584681600000001</v>
       </c>
       <c r="G17" s="1">
-        <v>17.600000000000001</v>
+        <f t="shared" si="2"/>
+        <v>17.418739686781194</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
@@ -1200,23 +3052,25 @@
         <v>14</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="C18" s="1">
-        <v>146.80000000000001</v>
+        <f>C10</f>
+        <v>220</v>
       </c>
       <c r="D18" s="1">
-        <v>2.4</v>
+        <f>D10</f>
+        <v>16.454000000000001</v>
       </c>
       <c r="E18" s="1">
-        <f>C18*D18</f>
-        <v>352.32</v>
+        <f>E10</f>
+        <v>3619.88</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
@@ -1224,22 +3078,25 @@
         <v>15</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C19" s="1">
-        <v>3208.4</v>
+        <f>SUM(C17:C18)</f>
+        <v>5220</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F19" s="1">
-        <v>1.8</v>
+        <f>SUM(E17:E18)/C19</f>
+        <v>11.789901915708812</v>
       </c>
       <c r="G19" s="1">
-        <v>20</v>
+        <f>((F19-$I$3)/$J$3)*100</f>
+        <v>20.810764298709032</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
@@ -1247,23 +3104,25 @@
         <v>16</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="C20" s="1">
-        <v>356</v>
+        <f>C14</f>
+        <v>2916.4</v>
       </c>
       <c r="D20" s="1">
-        <v>2.2000000000000002</v>
+        <f>D14</f>
+        <v>12.972</v>
       </c>
       <c r="E20" s="1">
-        <f>C20*D20</f>
-        <v>783.2</v>
+        <f>E14</f>
+        <v>37831.540800000002</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
@@ -1271,22 +3130,25 @@
         <v>17</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C21" s="1">
-        <v>3564.4</v>
+        <f>SUM(C19:C20)</f>
+        <v>8136.4</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F21" s="1">
-        <v>1.8</v>
+        <f>SUM(E17,E18,E20)/C21</f>
+        <v>12.213611523523918</v>
       </c>
       <c r="G21" s="1">
-        <v>23.5</v>
+        <f t="shared" ref="G21:G25" si="3">((F21-$I$3)/$J$3)*100</f>
+        <v>27.814132425568534</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
@@ -1294,23 +3156,25 @@
         <v>18</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="C22" s="1">
-        <v>756.5</v>
+        <f>C12</f>
+        <v>3500</v>
       </c>
       <c r="D22" s="1">
-        <v>1.7</v>
+        <f>D12</f>
+        <v>11.609712086917156</v>
       </c>
       <c r="E22" s="1">
-        <f>C22*D22</f>
-        <v>1286.05</v>
+        <f>E12</f>
+        <v>40633.992304210049</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
@@ -1318,22 +3182,25 @@
         <v>19</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C23" s="1">
-        <v>4320.8999999999996</v>
+        <f>SUM(C21:C22)</f>
+        <v>11636.4</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F23" s="1">
-        <v>1.8</v>
+        <f>SUM(E17,E18,E20,E22)/C23</f>
+        <v>12.031970463735352</v>
       </c>
       <c r="G23" s="1">
-        <v>21.8</v>
+        <f t="shared" si="3"/>
+        <v>24.811842212675057</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
@@ -1344,20 +3211,15 @@
         <v>5</v>
       </c>
       <c r="C24" s="1">
-        <v>311.5</v>
-      </c>
-      <c r="D24" s="1">
-        <v>1.7</v>
-      </c>
-      <c r="E24" s="1">
-        <f>C24*D24</f>
-        <v>529.54999999999995</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
       <c r="F24" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
@@ -1365,22 +3227,199 @@
         <v>21</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C25" s="1">
-        <v>4632.3999999999996</v>
+        <f>SUM(C23:C24)</f>
+        <v>11636.4</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F25" s="1">
-        <v>1.8</v>
+        <f>SUM(E17,E18,E20,E22,E24)/C25</f>
+        <v>12.031970463735352</v>
       </c>
       <c r="G25" s="1">
-        <v>21.3</v>
+        <f t="shared" si="3"/>
+        <v>24.811842212675057</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B28" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28">
+        <v>5000</v>
+      </c>
+      <c r="D28" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28">
+        <v>57923.408000000003</v>
+      </c>
+      <c r="F28">
+        <v>11.584681600000001</v>
+      </c>
+      <c r="G28">
+        <v>17.418739686781194</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29">
+        <v>2916.4</v>
+      </c>
+      <c r="D29">
+        <v>12.972</v>
+      </c>
+      <c r="E29">
+        <v>37831.540800000002</v>
+      </c>
+      <c r="F29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30">
+        <v>7916.4</v>
+      </c>
+      <c r="D30" t="s">
+        <v>13</v>
+      </c>
+      <c r="E30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F30">
+        <v>12.095769390126828</v>
+      </c>
+      <c r="G30">
+        <v>25.866355396650082</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B31" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31">
+        <v>3500</v>
+      </c>
+      <c r="D31">
+        <v>11.609712086917156</v>
+      </c>
+      <c r="E31">
+        <v>40633.992304210049</v>
+      </c>
+      <c r="F31" t="s">
+        <v>13</v>
+      </c>
+      <c r="G31" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B32" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32">
+        <v>11416.4</v>
+      </c>
+      <c r="D32" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32">
+        <v>11.946755641376447</v>
+      </c>
+      <c r="G32">
+        <v>23.403352152886814</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33">
+        <v>220</v>
+      </c>
+      <c r="D33">
+        <v>16.454000000000001</v>
+      </c>
+      <c r="E33">
+        <v>3619.88</v>
+      </c>
+      <c r="F33" t="s">
+        <v>13</v>
+      </c>
+      <c r="G33" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B34" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34">
+        <v>11636.4</v>
+      </c>
+      <c r="D34" t="s">
+        <v>13</v>
+      </c>
+      <c r="E34" t="s">
+        <v>13</v>
+      </c>
+      <c r="F34">
+        <v>12.031970463735355</v>
+      </c>
+      <c r="G34">
+        <v>24.811842212675113</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="F35" t="s">
+        <v>13</v>
+      </c>
+      <c r="G35" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B36" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36">
+        <v>11636.4</v>
+      </c>
+      <c r="D36" t="s">
+        <v>13</v>
+      </c>
+      <c r="E36" t="s">
+        <v>13</v>
+      </c>
+      <c r="F36">
+        <v>12.031970463735355</v>
+      </c>
+      <c r="G36">
+        <v>24.811842212675113</v>
       </c>
     </row>
   </sheetData>
@@ -1389,27 +3428,125 @@
     <mergeCell ref="A16:G16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{301EE39E-36B5-43F7-9622-90CD37749FCE}">
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.7265625" customWidth="1"/>
+    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="26">
+        <f>'Empty Weight'!B25</f>
+        <v>10.530833333333334</v>
+      </c>
+      <c r="B3" s="26">
+        <f>'Empty Weight'!C25</f>
+        <v>6.0500833333333333</v>
+      </c>
+      <c r="C3" s="8">
+        <f>17.42</f>
+        <v>17.420000000000002</v>
+      </c>
+      <c r="D3" s="8">
+        <v>25.87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C5">
+        <v>11.58</v>
+      </c>
+      <c r="D5">
+        <v>12.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>91</v>
+      </c>
+      <c r="B14" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="B15">
+        <f>B3*A15+A3</f>
+        <v>13.858379166666667</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A7:D7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="5e3388d9-314e-4294-86c7-b13e3e1771a6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DD955F58912B654AAA143FB6F23867BF" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ca35ef2c79184dece2382fe10a86ecc2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5e3388d9-314e-4294-86c7-b13e3e1771a6" xmlns:ns4="b7f6fc4a-4dd4-4733-a317-024af99a3eac" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="11badb3ba1486ac4ed64eef28c55e54c" ns3:_="" ns4:_="">
     <xsd:import namespace="5e3388d9-314e-4294-86c7-b13e3e1771a6"/>
@@ -1662,32 +3799,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84793EFF-49C1-4883-A0FB-581B72B07948}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="b7f6fc4a-4dd4-4733-a317-024af99a3eac"/>
-    <ds:schemaRef ds:uri="5e3388d9-314e-4294-86c7-b13e3e1771a6"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78904E1D-471D-4B0D-997C-93DA4375DA7A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="5e3388d9-314e-4294-86c7-b13e3e1771a6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{93CDCB7F-8648-4905-9D51-EA330003B102}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1704,4 +3833,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78904E1D-471D-4B0D-997C-93DA4375DA7A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84793EFF-49C1-4883-A0FB-581B72B07948}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="b7f6fc4a-4dd4-4733-a317-024af99a3eac"/>
+    <ds:schemaRef ds:uri="5e3388d9-314e-4294-86c7-b13e3e1771a6"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>